<commit_message>
the program now accepts any number of res files
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
         <v>2.996145142857143</v>
       </c>
       <c r="D2" t="n">
-        <v>4021.08610295068</v>
+        <v>40210.8610295068</v>
       </c>
       <c r="E2" t="n">
         <v>29.48833428571428</v>
@@ -495,7 +495,7 @@
         <v>3.308152777777777</v>
       </c>
       <c r="D3" t="n">
-        <v>4402.551001771774</v>
+        <v>44025.51001771774</v>
       </c>
       <c r="E3" t="n">
         <v>36.4758275</v>
@@ -517,7 +517,7 @@
         <v>4.395085135135135</v>
       </c>
       <c r="D4" t="n">
-        <v>5835.583396856042</v>
+        <v>58355.83396856042</v>
       </c>
       <c r="E4" t="n">
         <v>64.48898486486488</v>
@@ -529,139 +529,139 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>Placa_1 1</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9473532113458141</v>
+        <v>0.5171329573658486</v>
       </c>
       <c r="C5" t="n">
-        <v>5.489527222222224</v>
+        <v>2.996145142857143</v>
       </c>
       <c r="D5" t="n">
-        <v>7242.62339645898</v>
+        <v>40210.8610295068</v>
       </c>
       <c r="E5" t="n">
-        <v>100.8328161111111</v>
+        <v>29.48833428571428</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2417405763006262</v>
+        <v>0.09439878676581151</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>Placa_3 1</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.140045356010704</v>
+        <v>0.5171329573658486</v>
       </c>
       <c r="C6" t="n">
-        <v>6.606468285714286</v>
+        <v>2.996145142857143</v>
       </c>
       <c r="D6" t="n">
-        <v>8657.173739163705</v>
+        <v>40210.8610295068</v>
       </c>
       <c r="E6" t="n">
-        <v>145.9750517142857</v>
+        <v>29.48833428571428</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3444630314620629</v>
+        <v>0.09439878676581151</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Placa_1 1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.5171329573658486</v>
+        <v>0.5709444553684897</v>
       </c>
       <c r="C7" t="n">
-        <v>2.996145142857143</v>
+        <v>3.308152777777777</v>
       </c>
       <c r="D7" t="n">
-        <v>4021.08610295068</v>
+        <v>44025.51001771774</v>
       </c>
       <c r="E7" t="n">
-        <v>29.48833428571428</v>
+        <v>36.4758275</v>
       </c>
       <c r="F7" t="n">
-        <v>0.09439878676581151</v>
+        <v>0.1039381158842682</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5709444553684897</v>
+        <v>0.7585202529229677</v>
       </c>
       <c r="C8" t="n">
-        <v>3.308152777777777</v>
+        <v>4.395085135135135</v>
       </c>
       <c r="D8" t="n">
-        <v>4402.551001771774</v>
+        <v>58355.83396856042</v>
       </c>
       <c r="E8" t="n">
-        <v>36.4758275</v>
+        <v>64.48898486486488</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1039381158842682</v>
+        <v>0.1992425198041262</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.7585202529229677</v>
+        <v>0.9473532113458141</v>
       </c>
       <c r="C9" t="n">
-        <v>4.395085135135135</v>
+        <v>5.489527222222224</v>
       </c>
       <c r="D9" t="n">
-        <v>5835.583396856042</v>
+        <v>72426.23396458979</v>
       </c>
       <c r="E9" t="n">
-        <v>64.48898486486488</v>
+        <v>100.8328161111111</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1992425198041262</v>
+        <v>0.2417405763006262</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9473532113458141</v>
+        <v>1.140045356010704</v>
       </c>
       <c r="C10" t="n">
-        <v>5.489527222222224</v>
+        <v>6.606468285714286</v>
       </c>
       <c r="D10" t="n">
-        <v>7242.62339645898</v>
+        <v>86571.73739163704</v>
       </c>
       <c r="E10" t="n">
-        <v>100.8328161111111</v>
+        <v>145.9750517142857</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2417405763006262</v>
+        <v>0.3444630314620629</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -671,7 +671,7 @@
         <v>6.606468285714286</v>
       </c>
       <c r="D11" t="n">
-        <v>8657.173739163705</v>
+        <v>86571.73739163704</v>
       </c>
       <c r="E11" t="n">
         <v>145.9750517142857</v>
@@ -683,110 +683,22 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Placa_3 1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.5171329573658486</v>
+        <v>1.140045356010704</v>
       </c>
       <c r="C12" t="n">
-        <v>2.996145142857143</v>
+        <v>6.606468285714286</v>
       </c>
       <c r="D12" t="n">
-        <v>4021.08610295068</v>
+        <v>86571.73739163704</v>
       </c>
       <c r="E12" t="n">
-        <v>29.48833428571428</v>
+        <v>145.9750517142857</v>
       </c>
       <c r="F12" t="n">
-        <v>0.09439878676581151</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>0.5709444553684897</v>
-      </c>
-      <c r="C13" t="n">
-        <v>3.308152777777777</v>
-      </c>
-      <c r="D13" t="n">
-        <v>4402.551001771774</v>
-      </c>
-      <c r="E13" t="n">
-        <v>36.4758275</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.1039381158842682</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>0.7585202529229677</v>
-      </c>
-      <c r="C14" t="n">
-        <v>4.395085135135135</v>
-      </c>
-      <c r="D14" t="n">
-        <v>5835.583396856042</v>
-      </c>
-      <c r="E14" t="n">
-        <v>64.48898486486488</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.1992425198041262</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>0.9473532113458141</v>
-      </c>
-      <c r="C15" t="n">
-        <v>5.489527222222224</v>
-      </c>
-      <c r="D15" t="n">
-        <v>7242.62339645898</v>
-      </c>
-      <c r="E15" t="n">
-        <v>100.8328161111111</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.2417405763006262</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>1.140045356010704</v>
-      </c>
-      <c r="C16" t="n">
-        <v>6.606468285714286</v>
-      </c>
-      <c r="D16" t="n">
-        <v>8657.173739163705</v>
-      </c>
-      <c r="E16" t="n">
-        <v>145.9750517142857</v>
-      </c>
-      <c r="F16" t="n">
         <v>0.3444630314620629</v>
       </c>
     </row>

</xml_diff>